<commit_message>
Level 1 + 2bmp
template and lvl 1 complete, lvl 2 waiting for array conversion
</commit_message>
<xml_diff>
--- a/Puzzles/Level 1.xlsx
+++ b/Puzzles/Level 1.xlsx
@@ -16,6 +16,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="4">
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>bed</t>
+  </si>
+  <si>
+    <t>hooman</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -49,8 +66,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,12 +351,401 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>